<commit_message>
Datos utilizados en actualización de evaluación de stock de sardina austral Los lagos (25/8/2021)
</commit_message>
<xml_diff>
--- a/Datos_a_Junio/DESEMBARQUE.xlsx
+++ b/Datos_a_Junio/DESEMBARQUE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/CTP2021/SARDINA_AUSTRAL LOS LAGOS/INFORME_FINAL/Datos_a_Junio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/CTP2022/SARDINAAUSTRAL_LAGOS/PRIMER_INFORME/Datos_a_Junio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9086448A-D4B6-2A44-8F21-E8C239C7B294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D7EB17-B798-984B-AF5E-F8BFC9BA6036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17040" yWindow="880" windowWidth="25340" windowHeight="26820" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
+    <workbookView xWindow="23580" yWindow="500" windowWidth="25340" windowHeight="26820" activeTab="1" xr2:uid="{D73FE552-5237-42B3-AA1B-489DDDA3A168}"/>
   </bookViews>
   <sheets>
     <sheet name="XI Region " sheetId="2" r:id="rId1"/>
@@ -4740,7 +4740,7 @@
   </sheetPr>
   <dimension ref="B2:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -5169,8 +5169,8 @@
   </sheetPr>
   <dimension ref="B2:AD64"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="W42" sqref="W42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>